<commit_message>
Fix LLM Validation Result.
</commit_message>
<xml_diff>
--- a/docs/samples/Pre-Approval/Case2_GPT_Result.xlsx
+++ b/docs/samples/Pre-Approval/Case2_GPT_Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work DRT\ULINK\AI Claim Pre-Approval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ulink-is-ai\docs\samples\Pre-Approval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA5532E-F633-4458-92FD-D986338861E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259D98A4-C2C1-4563-856A-8FDA95B1EF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="5535" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{38014062-9CD7-4D3E-B7B3-B0E986C6407F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{38014062-9CD7-4D3E-B7B3-B0E986C6407F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Sheet" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B658CF84-F10A-43F6-9495-930B5311C797}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="255.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,49 +664,49 @@
       <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>31088</v>
-      </c>
-      <c r="G2" s="1">
-        <v>45368</v>
       </c>
       <c r="H2" s="1">
         <v>45368</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1">
+        <v>45368</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>108700</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>41</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>108700</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>42</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>43</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -782,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0DD1FC-9CAE-4453-9202-6766F55237DF}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>